<commit_message>
now it works only by python
</commit_message>
<xml_diff>
--- a/methods.xlsx
+++ b/methods.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="115">
+  <si>
+    <t xml:space="preserve">METHOD_NAMES</t>
+  </si>
   <si>
     <t xml:space="preserve">Java</t>
   </si>
@@ -371,7 +374,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -395,8 +398,10 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -425,12 +430,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="alias"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="5">
@@ -500,7 +499,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -574,10 +573,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -672,8 +667,8 @@
   </sheetPr>
   <dimension ref="A1:K975"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -684,56 +679,59 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -747,17 +745,17 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
@@ -768,17 +766,17 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
@@ -789,15 +787,15 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="8"/>
       <c r="E6" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
@@ -808,7 +806,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="14"/>
@@ -823,19 +821,19 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>23</v>
-      </c>
       <c r="D8" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
@@ -846,19 +844,19 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
@@ -869,7 +867,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -884,7 +882,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -899,7 +897,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -914,16 +912,16 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="10"/>
@@ -935,7 +933,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -950,7 +948,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="5"/>
@@ -965,16 +963,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E16" s="15"/>
       <c r="F16" s="10"/>
@@ -986,7 +984,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -1001,14 +999,14 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E18" s="15"/>
       <c r="F18" s="10"/>
@@ -1020,16 +1018,16 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E19" s="15"/>
       <c r="F19" s="10"/>
@@ -1041,16 +1039,16 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E20" s="15"/>
       <c r="F20" s="10"/>
@@ -1062,16 +1060,16 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E21" s="15"/>
       <c r="F21" s="10"/>
@@ -1083,16 +1081,16 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E22" s="15"/>
       <c r="F22" s="10"/>
@@ -1104,17 +1102,17 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
@@ -1125,7 +1123,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -1140,19 +1138,19 @@
     </row>
     <row r="25" customFormat="false" ht="24.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
@@ -1163,15 +1161,15 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
@@ -1182,10 +1180,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C27" s="14"/>
       <c r="D27" s="8"/>
@@ -1199,19 +1197,19 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
@@ -1222,16 +1220,16 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>67</v>
-      </c>
       <c r="D29" s="13" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
@@ -1242,17 +1240,17 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
@@ -1263,19 +1261,19 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
@@ -1286,19 +1284,19 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
@@ -1309,19 +1307,19 @@
     </row>
     <row r="33" customFormat="false" ht="24.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="E33" s="19" t="s">
         <v>81</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>82</v>
       </c>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
@@ -1332,17 +1330,17 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
@@ -1353,17 +1351,17 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
@@ -1374,17 +1372,17 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
@@ -1395,19 +1393,19 @@
     </row>
     <row r="37" customFormat="false" ht="24.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
@@ -1418,19 +1416,19 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
@@ -1441,17 +1439,17 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
@@ -1462,17 +1460,17 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="17" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F40" s="10"/>
       <c r="G40" s="10"/>
@@ -1483,19 +1481,19 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="B41" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="C41" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="D41" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="E41" s="21" t="s">
-        <v>108</v>
+        <v>109</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>109</v>
       </c>
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
@@ -1506,7 +1504,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="16" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B42" s="16"/>
       <c r="C42" s="16"/>
@@ -1521,7 +1519,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="16" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B43" s="16"/>
       <c r="C43" s="16"/>
@@ -1536,7 +1534,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="16" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B44" s="16"/>
       <c r="C44" s="16"/>
@@ -1551,15 +1549,15 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="B45" s="22"/>
-      <c r="C45" s="22"/>
+        <v>113</v>
+      </c>
+      <c r="B45" s="21"/>
+      <c r="C45" s="21"/>
       <c r="D45" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="E45" s="16" t="s">
         <v>113</v>
-      </c>
-      <c r="E45" s="16" t="s">
-        <v>112</v>
       </c>
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>

</xml_diff>